<commit_message>
Minor correction to Marthas localmap summary
</commit_message>
<xml_diff>
--- a/redisProcess/ineRedist2017/origen distritaciones locales.xlsx
+++ b/redisProcess/ineRedist2017/origen distritaciones locales.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">consenso</t>
   </si>
   <si>
-    <t xml:space="preserve">Colima*</t>
+    <t xml:space="preserve">Colima</t>
   </si>
   <si>
     <t xml:space="preserve">Escenario alterno propuesto por la DERFE por recomendación del CTD</t>
@@ -422,7 +422,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -447,26 +447,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,20 +471,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -539,7 +515,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -612,17 +588,17 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -690,13 +666,13 @@
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -710,10 +686,10 @@
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -736,13 +712,13 @@
       <c r="C6" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -753,13 +729,13 @@
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -770,10 +746,10 @@
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -807,40 +783,40 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="n">
+      <c r="C11" s="6" t="n">
         <v>2017</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -854,7 +830,7 @@
       <c r="C12" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -868,10 +844,10 @@
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -888,19 +864,19 @@
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -928,10 +904,10 @@
       <c r="A16" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>2017</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -948,13 +924,13 @@
       <c r="A17" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -968,54 +944,54 @@
       <c r="A18" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="13" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D19" s="19" t="s">
+      <c r="C19" s="10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="15" t="n">
+      <c r="C20" s="6" t="n">
         <v>2017</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -1026,7 +1002,7 @@
       <c r="A21" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="4" t="n">
@@ -1046,10 +1022,10 @@
       <c r="A22" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1072,7 +1048,7 @@
       <c r="C23" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1092,7 +1068,7 @@
       <c r="C24" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1146,10 +1122,10 @@
       <c r="A27" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1186,19 +1162,19 @@
       <c r="A29" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1226,10 +1202,10 @@
       <c r="A31" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="6" t="n">
         <v>2017</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -1246,10 +1222,10 @@
       <c r="A32" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="7" t="n">
+      <c r="C32" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1295,10 +1271,10 @@
       <c r="D34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1326,39 +1302,39 @@
       <c r="A36" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="7" t="n">
+      <c r="C36" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="n">
+      <c r="A37" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="23" t="n">
-        <v>2015</v>
-      </c>
-      <c r="D37" s="24" t="s">
+      <c r="C37" s="17" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="20" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Discards two commits, adds minor correction to Marthas loc summary and sanLoc map
</commit_message>
<xml_diff>
--- a/redisProcess/ineRedist2017/origen distritaciones locales.xlsx
+++ b/redisProcess/ineRedist2017/origen distritaciones locales.xlsx
@@ -84,7 +84,7 @@
     <t xml:space="preserve">consenso</t>
   </si>
   <si>
-    <t xml:space="preserve">Colima*</t>
+    <t xml:space="preserve">Colima</t>
   </si>
   <si>
     <t xml:space="preserve">Escenario alterno propuesto por la DERFE por recomendación del CTD</t>
@@ -422,7 +422,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -447,26 +447,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -483,20 +471,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -539,7 +515,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -612,17 +588,17 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.9919028340081"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -690,13 +666,13 @@
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -710,10 +686,10 @@
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -736,13 +712,13 @@
       <c r="C6" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -753,13 +729,13 @@
       <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -770,10 +746,10 @@
       <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D8" s="5" t="s">
@@ -807,40 +783,40 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="C10" s="10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="n">
+      <c r="C11" s="6" t="n">
         <v>2017</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -854,7 +830,7 @@
       <c r="C12" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="12" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -868,10 +844,10 @@
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -888,19 +864,19 @@
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="C14" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -928,10 +904,10 @@
       <c r="A16" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="6" t="n">
         <v>2017</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -948,13 +924,13 @@
       <c r="A17" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D17" s="17" t="s">
+      <c r="C17" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -968,54 +944,54 @@
       <c r="A18" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="7" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="C18" s="6" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="10" t="s">
+      <c r="E18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="13" t="n">
-        <v>2016</v>
-      </c>
-      <c r="D19" s="19" t="s">
+      <c r="C19" s="10" t="n">
+        <v>2016</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="35.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="15" t="n">
+      <c r="C20" s="6" t="n">
         <v>2017</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="2" t="s">
@@ -1026,7 +1002,7 @@
       <c r="A21" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="3" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="4" t="n">
@@ -1046,10 +1022,10 @@
       <c r="A22" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D22" s="5" t="s">
@@ -1072,7 +1048,7 @@
       <c r="C23" s="4" t="n">
         <v>2015</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -1092,7 +1068,7 @@
       <c r="C24" s="4" t="n">
         <v>2017</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E24" s="2" t="s">
@@ -1146,10 +1122,10 @@
       <c r="A27" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D27" s="5" t="s">
@@ -1186,19 +1162,19 @@
       <c r="A29" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1226,10 +1202,10 @@
       <c r="A31" s="2" t="n">
         <v>26</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="6" t="n">
         <v>2017</v>
       </c>
       <c r="D31" s="5" t="s">
@@ -1246,10 +1222,10 @@
       <c r="A32" s="2" t="n">
         <v>27</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C32" s="7" t="n">
+      <c r="C32" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1295,10 +1271,10 @@
       <c r="D34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1326,39 +1302,39 @@
       <c r="A36" s="2" t="n">
         <v>31</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="7" t="n">
+      <c r="C36" s="6" t="n">
         <v>2016</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="19.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="21" t="n">
+      <c r="A37" s="15" t="n">
         <v>32</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="23" t="n">
-        <v>2015</v>
-      </c>
-      <c r="D37" s="24" t="s">
+      <c r="C37" s="17" t="n">
+        <v>2015</v>
+      </c>
+      <c r="D37" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F37" s="20" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>